<commit_message>
modify ntc and temperature accuracy
</commit_message>
<xml_diff>
--- a/air_condition/docs/工作簿1.xlsx
+++ b/air_condition/docs/工作簿1.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24860" windowHeight="9660"/>
+    <workbookView windowWidth="24860" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="HR202L" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -34,12 +34,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="176" formatCode="@&quot;,&quot;"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="@,"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.0_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="@&quot;,&quot;"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -65,53 +65,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,6 +81,51 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -134,15 +133,39 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,9 +186,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,7 +195,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,28 +203,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,25 +223,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,31 +241,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +259,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,55 +271,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,25 +289,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,13 +337,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,8 +457,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -472,28 +472,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,6 +497,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -524,15 +522,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -551,129 +540,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -682,40 +682,37 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -726,7 +723,7 @@
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2871,7 +2868,7 @@
   <sheetPr/>
   <dimension ref="C1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
+    <sheetView topLeftCell="C133" workbookViewId="0">
       <selection activeCell="L133" sqref="L$1:L$1048576"/>
     </sheetView>
   </sheetViews>
@@ -2888,16 +2885,16 @@
       <c r="C1" s="4">
         <v>190.5562</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4">
         <f>C1*10000</f>
         <v>1905562</v>
       </c>
-      <c r="E1" s="7" t="str">
+      <c r="E1" s="6" t="str">
         <f>DEC2HEX(D1)</f>
         <v>1D139A</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9">
+      <c r="F1" s="7"/>
+      <c r="G1" s="8">
         <v>-40</v>
       </c>
     </row>
@@ -2905,16 +2902,16 @@
       <c r="C2" s="4">
         <v>183.4132</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <f t="shared" ref="D2:D33" si="0">C2*10000</f>
         <v>1834132</v>
       </c>
-      <c r="E2" s="7" t="str">
+      <c r="E2" s="6" t="str">
         <f t="shared" ref="E2:E33" si="1">DEC2HEX(D2)</f>
         <v>1BFC94</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8">
         <f>G1+1</f>
         <v>-39</v>
       </c>
@@ -2923,16 +2920,16 @@
       <c r="C3" s="4">
         <v>175.674</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <f t="shared" si="0"/>
         <v>1756740</v>
       </c>
-      <c r="E3" s="7" t="str">
+      <c r="E3" s="6" t="str">
         <f t="shared" si="1"/>
         <v>1ACE44</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9">
+      <c r="F3" s="7"/>
+      <c r="G3" s="8">
         <f t="shared" ref="G3:G34" si="2">G2+1</f>
         <v>-38</v>
       </c>
@@ -2941,16 +2938,16 @@
       <c r="C4" s="4">
         <v>167.6467</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>1676467</v>
       </c>
-      <c r="E4" s="7" t="str">
+      <c r="E4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>1994B3</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9">
+      <c r="F4" s="7"/>
+      <c r="G4" s="8">
         <f t="shared" si="2"/>
         <v>-37</v>
       </c>
@@ -2959,16 +2956,16 @@
       <c r="C5" s="4">
         <v>159.5647</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <f t="shared" si="0"/>
         <v>1595647</v>
       </c>
-      <c r="E5" s="7" t="str">
+      <c r="E5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>1858FF</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9">
+      <c r="F5" s="7"/>
+      <c r="G5" s="8">
         <f t="shared" si="2"/>
         <v>-36</v>
       </c>
@@ -2977,16 +2974,16 @@
       <c r="C6" s="4">
         <v>151.5975</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f t="shared" si="0"/>
         <v>1515975</v>
       </c>
-      <c r="E6" s="7" t="str">
+      <c r="E6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>1721C7</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9">
+      <c r="F6" s="7"/>
+      <c r="G6" s="8">
         <f t="shared" si="2"/>
         <v>-35</v>
       </c>
@@ -2995,16 +2992,16 @@
       <c r="C7" s="4">
         <v>143.8624</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <f t="shared" si="0"/>
         <v>1438624</v>
       </c>
-      <c r="E7" s="7" t="str">
+      <c r="E7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>15F3A0</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9">
+      <c r="F7" s="7"/>
+      <c r="G7" s="8">
         <f t="shared" si="2"/>
         <v>-34</v>
       </c>
@@ -3013,16 +3010,16 @@
       <c r="C8" s="4">
         <v>136.4361</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <f t="shared" si="0"/>
         <v>1364361</v>
       </c>
-      <c r="E8" s="7" t="str">
+      <c r="E8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>14D189</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9">
+      <c r="F8" s="7"/>
+      <c r="G8" s="8">
         <f t="shared" si="2"/>
         <v>-33</v>
       </c>
@@ -3031,16 +3028,16 @@
       <c r="C9" s="4">
         <v>129.3641</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>1293641</v>
       </c>
-      <c r="E9" s="7" t="str">
+      <c r="E9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13BD49</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9">
+      <c r="F9" s="7"/>
+      <c r="G9" s="8">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -3049,16 +3046,16 @@
       <c r="C10" s="4">
         <v>122.6678</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <f t="shared" si="0"/>
         <v>1226678</v>
       </c>
-      <c r="E10" s="7" t="str">
+      <c r="E10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>12B7B6</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9">
+      <c r="F10" s="7"/>
+      <c r="G10" s="8">
         <f t="shared" si="2"/>
         <v>-31</v>
       </c>
@@ -3067,16 +3064,16 @@
       <c r="C11" s="4">
         <v>116.3519</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f t="shared" si="0"/>
         <v>1163519</v>
       </c>
-      <c r="E11" s="7" t="str">
+      <c r="E11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>11C0FF</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9">
+      <c r="F11" s="7"/>
+      <c r="G11" s="8">
         <f t="shared" si="2"/>
         <v>-30</v>
       </c>
@@ -3085,16 +3082,16 @@
       <c r="C12" s="4">
         <v>110.4098</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <f t="shared" si="0"/>
         <v>1104098</v>
       </c>
-      <c r="E12" s="7" t="str">
+      <c r="E12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>10D8E2</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9">
+      <c r="F12" s="7"/>
+      <c r="G12" s="8">
         <f t="shared" si="2"/>
         <v>-29</v>
       </c>
@@ -3103,34 +3100,34 @@
       <c r="C13" s="4">
         <v>104.8272</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <f t="shared" si="0"/>
         <v>1048272</v>
       </c>
-      <c r="E13" s="7" t="str">
+      <c r="E13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>FFED0</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9">
+      <c r="F13" s="7"/>
+      <c r="G13" s="8">
         <f t="shared" si="2"/>
         <v>-28</v>
       </c>
     </row>
     <row r="14" spans="3:7">
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>99.5847</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <f t="shared" si="0"/>
         <v>995847</v>
       </c>
-      <c r="E14" s="7" t="str">
+      <c r="E14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>F3207</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9">
+      <c r="F14" s="7"/>
+      <c r="G14" s="8">
         <f t="shared" si="2"/>
         <v>-27</v>
       </c>
@@ -3139,16 +3136,16 @@
       <c r="C15" s="4">
         <v>94.6608</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f t="shared" si="0"/>
         <v>946608</v>
       </c>
-      <c r="E15" s="7" t="str">
+      <c r="E15" s="6" t="str">
         <f t="shared" si="1"/>
         <v>E71B0</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9">
+      <c r="F15" s="7"/>
+      <c r="G15" s="8">
         <f t="shared" si="2"/>
         <v>-26</v>
       </c>
@@ -3157,16 +3154,16 @@
       <c r="C16" s="4">
         <v>90.0326</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <f t="shared" si="0"/>
         <v>900326</v>
       </c>
-      <c r="E16" s="7" t="str">
+      <c r="E16" s="6" t="str">
         <f t="shared" si="1"/>
         <v>DBCE6</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9">
+      <c r="F16" s="7"/>
+      <c r="G16" s="8">
         <f t="shared" si="2"/>
         <v>-25</v>
       </c>
@@ -3175,16 +3172,16 @@
       <c r="C17" s="4">
         <v>85.6778</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <f t="shared" si="0"/>
         <v>856778</v>
       </c>
-      <c r="E17" s="7" t="str">
+      <c r="E17" s="6" t="str">
         <f t="shared" si="1"/>
         <v>D12CA</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9">
+      <c r="F17" s="7"/>
+      <c r="G17" s="8">
         <f t="shared" si="2"/>
         <v>-24</v>
       </c>
@@ -3193,16 +3190,16 @@
       <c r="C18" s="4">
         <v>81.5747</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <f t="shared" si="0"/>
         <v>815747</v>
       </c>
-      <c r="E18" s="7" t="str">
+      <c r="E18" s="6" t="str">
         <f t="shared" si="1"/>
         <v>C7283</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9">
+      <c r="F18" s="7"/>
+      <c r="G18" s="8">
         <f t="shared" si="2"/>
         <v>-23</v>
       </c>
@@ -3211,16 +3208,16 @@
       <c r="C19" s="4">
         <v>77.7031</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <f t="shared" si="0"/>
         <v>777031</v>
       </c>
-      <c r="E19" s="7" t="str">
+      <c r="E19" s="6" t="str">
         <f t="shared" si="1"/>
         <v>BDB47</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9">
+      <c r="F19" s="7"/>
+      <c r="G19" s="8">
         <f t="shared" si="2"/>
         <v>-22</v>
       </c>
@@ -3229,16 +3226,16 @@
       <c r="C20" s="4">
         <v>74.0442</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <f t="shared" si="0"/>
         <v>740442</v>
       </c>
-      <c r="E20" s="7" t="str">
+      <c r="E20" s="6" t="str">
         <f t="shared" si="1"/>
         <v>B4C5A</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9">
+      <c r="F20" s="7"/>
+      <c r="G20" s="8">
         <f t="shared" si="2"/>
         <v>-21</v>
       </c>
@@ -3247,16 +3244,16 @@
       <c r="C21" s="4">
         <v>70.5811</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <f t="shared" si="0"/>
         <v>705811</v>
       </c>
-      <c r="E21" s="7" t="str">
+      <c r="E21" s="6" t="str">
         <f t="shared" si="1"/>
         <v>AC513</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9">
+      <c r="F21" s="7"/>
+      <c r="G21" s="8">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
@@ -3265,16 +3262,16 @@
       <c r="C22" s="4">
         <v>67.2987</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <f t="shared" si="0"/>
         <v>672987</v>
       </c>
-      <c r="E22" s="7" t="str">
+      <c r="E22" s="6" t="str">
         <f t="shared" si="1"/>
         <v>A44DB</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9">
+      <c r="F22" s="7"/>
+      <c r="G22" s="8">
         <f t="shared" si="2"/>
         <v>-19</v>
       </c>
@@ -3283,16 +3280,16 @@
       <c r="C23" s="4">
         <v>64.1834</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <f t="shared" si="0"/>
         <v>641834</v>
       </c>
-      <c r="E23" s="7" t="str">
+      <c r="E23" s="6" t="str">
         <f t="shared" si="1"/>
         <v>9CB2A</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9">
+      <c r="F23" s="7"/>
+      <c r="G23" s="8">
         <f t="shared" si="2"/>
         <v>-18</v>
       </c>
@@ -3301,16 +3298,16 @@
       <c r="C24" s="4">
         <v>61.2233</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <f t="shared" si="0"/>
         <v>612233</v>
       </c>
-      <c r="E24" s="7" t="str">
+      <c r="E24" s="6" t="str">
         <f t="shared" si="1"/>
         <v>95789</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="9">
+      <c r="F24" s="7"/>
+      <c r="G24" s="8">
         <f t="shared" si="2"/>
         <v>-17</v>
       </c>
@@ -3319,16 +3316,16 @@
       <c r="C25" s="4">
         <v>58.408</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <f t="shared" si="0"/>
         <v>584080</v>
       </c>
-      <c r="E25" s="7" t="str">
+      <c r="E25" s="6" t="str">
         <f t="shared" si="1"/>
         <v>8E990</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9">
+      <c r="F25" s="7"/>
+      <c r="G25" s="8">
         <f t="shared" si="2"/>
         <v>-16</v>
       </c>
@@ -3337,34 +3334,34 @@
       <c r="C26" s="4">
         <v>55.7284</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <f t="shared" si="0"/>
         <v>557284</v>
       </c>
-      <c r="E26" s="7" t="str">
+      <c r="E26" s="6" t="str">
         <f t="shared" si="1"/>
         <v>880E4</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="9">
+      <c r="F26" s="7"/>
+      <c r="G26" s="8">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
     </row>
     <row r="27" spans="3:7">
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>53.1766</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <f t="shared" si="0"/>
         <v>531766</v>
       </c>
-      <c r="E27" s="7" t="str">
+      <c r="E27" s="6" t="str">
         <f t="shared" si="1"/>
         <v>81D36</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="9">
+      <c r="F27" s="7"/>
+      <c r="G27" s="8">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
@@ -3373,16 +3370,16 @@
       <c r="C28" s="4">
         <v>50.7456</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <f t="shared" si="0"/>
         <v>507456</v>
       </c>
-      <c r="E28" s="7" t="str">
+      <c r="E28" s="6" t="str">
         <f t="shared" si="1"/>
         <v>7BE40</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9">
+      <c r="F28" s="7"/>
+      <c r="G28" s="8">
         <f t="shared" si="2"/>
         <v>-13</v>
       </c>
@@ -3391,16 +3388,16 @@
       <c r="C29" s="4">
         <v>48.4294</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <f t="shared" si="0"/>
         <v>484294</v>
       </c>
-      <c r="E29" s="7" t="str">
+      <c r="E29" s="6" t="str">
         <f t="shared" si="1"/>
         <v>763C6</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="9">
+      <c r="F29" s="7"/>
+      <c r="G29" s="8">
         <f t="shared" si="2"/>
         <v>-12</v>
       </c>
@@ -3409,16 +3406,16 @@
       <c r="C30" s="4">
         <v>46.2224</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <f t="shared" si="0"/>
         <v>462224</v>
       </c>
-      <c r="E30" s="7" t="str">
+      <c r="E30" s="6" t="str">
         <f t="shared" si="1"/>
         <v>70D90</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="9">
+      <c r="F30" s="7"/>
+      <c r="G30" s="8">
         <f t="shared" si="2"/>
         <v>-11</v>
       </c>
@@ -3427,16 +3424,16 @@
       <c r="C31" s="4">
         <v>44.1201</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <f t="shared" si="0"/>
         <v>441201</v>
       </c>
-      <c r="E31" s="7" t="str">
+      <c r="E31" s="6" t="str">
         <f t="shared" si="1"/>
         <v>6BB71</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9">
+      <c r="F31" s="7"/>
+      <c r="G31" s="8">
         <f t="shared" si="2"/>
         <v>-10</v>
       </c>
@@ -3445,16 +3442,16 @@
       <c r="C32" s="4">
         <v>42.118</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <f t="shared" si="0"/>
         <v>421180</v>
       </c>
-      <c r="E32" s="7" t="str">
+      <c r="E32" s="6" t="str">
         <f t="shared" si="1"/>
         <v>66D3C</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9">
+      <c r="F32" s="7"/>
+      <c r="G32" s="8">
         <f t="shared" si="2"/>
         <v>-9</v>
       </c>
@@ -3463,16 +3460,16 @@
       <c r="C33" s="4">
         <v>40.2121</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <f t="shared" si="0"/>
         <v>402121</v>
       </c>
-      <c r="E33" s="7" t="str">
+      <c r="E33" s="6" t="str">
         <f t="shared" si="1"/>
         <v>622C9</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9">
+      <c r="F33" s="7"/>
+      <c r="G33" s="8">
         <f t="shared" si="2"/>
         <v>-8</v>
       </c>
@@ -3481,16 +3478,16 @@
       <c r="C34" s="4">
         <v>38.3988</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="4">
         <f t="shared" ref="D34:D65" si="3">C34*10000</f>
         <v>383988</v>
       </c>
-      <c r="E34" s="7" t="str">
+      <c r="E34" s="6" t="str">
         <f t="shared" ref="E34:E65" si="4">DEC2HEX(D34)</f>
         <v>5DBF4</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9">
+      <c r="F34" s="7"/>
+      <c r="G34" s="8">
         <f t="shared" si="2"/>
         <v>-7</v>
       </c>
@@ -3499,16 +3496,16 @@
       <c r="C35" s="4">
         <v>36.6746</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <f t="shared" si="3"/>
         <v>366746</v>
       </c>
-      <c r="E35" s="7" t="str">
+      <c r="E35" s="6" t="str">
         <f t="shared" si="4"/>
         <v>5989A</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9">
+      <c r="F35" s="7"/>
+      <c r="G35" s="8">
         <f t="shared" ref="G35:G66" si="5">G34+1</f>
         <v>-6</v>
       </c>
@@ -3517,16 +3514,16 @@
       <c r="C36" s="4">
         <v>35.0362</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="4">
         <f t="shared" si="3"/>
         <v>350362</v>
       </c>
-      <c r="E36" s="7" t="str">
+      <c r="E36" s="6" t="str">
         <f t="shared" si="4"/>
         <v>5589A</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="9">
+      <c r="F36" s="7"/>
+      <c r="G36" s="8">
         <f t="shared" si="5"/>
         <v>-5</v>
       </c>
@@ -3535,16 +3532,16 @@
       <c r="C37" s="4">
         <v>33.4802</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="4">
         <f t="shared" si="3"/>
         <v>334802</v>
       </c>
-      <c r="E37" s="7" t="str">
+      <c r="E37" s="6" t="str">
         <f t="shared" si="4"/>
         <v>51BD2</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="9">
+      <c r="F37" s="7"/>
+      <c r="G37" s="8">
         <f t="shared" si="5"/>
         <v>-4</v>
       </c>
@@ -3553,16 +3550,16 @@
       <c r="C38" s="4">
         <v>32.0035</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="4">
         <f t="shared" si="3"/>
         <v>320035</v>
       </c>
-      <c r="E38" s="7" t="str">
+      <c r="E38" s="6" t="str">
         <f t="shared" si="4"/>
         <v>4E223</v>
       </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="9">
+      <c r="F38" s="7"/>
+      <c r="G38" s="8">
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
@@ -3571,34 +3568,34 @@
       <c r="C39" s="4">
         <v>30.6028</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="4">
         <f t="shared" si="3"/>
         <v>306028</v>
       </c>
-      <c r="E39" s="7" t="str">
+      <c r="E39" s="6" t="str">
         <f t="shared" si="4"/>
         <v>4AB6C</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="9">
+      <c r="F39" s="7"/>
+      <c r="G39" s="8">
         <f t="shared" si="5"/>
         <v>-2</v>
       </c>
     </row>
     <row r="40" spans="3:7">
-      <c r="C40" s="6">
+      <c r="C40" s="5">
         <v>29.275</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="4">
         <f t="shared" si="3"/>
         <v>292750</v>
       </c>
-      <c r="E40" s="7" t="str">
+      <c r="E40" s="6" t="str">
         <f t="shared" si="4"/>
         <v>4778E</v>
       </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="9">
+      <c r="F40" s="7"/>
+      <c r="G40" s="8">
         <f t="shared" si="5"/>
         <v>-1</v>
       </c>
@@ -3607,16 +3604,16 @@
       <c r="C41" s="4">
         <v>28.017</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="4">
         <f t="shared" si="3"/>
         <v>280170</v>
       </c>
-      <c r="E41" s="7" t="str">
+      <c r="E41" s="6" t="str">
         <f t="shared" si="4"/>
         <v>4466A</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="9">
+      <c r="F41" s="7"/>
+      <c r="G41" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3625,16 +3622,16 @@
       <c r="C42" s="4">
         <v>26.8255</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="4">
         <f t="shared" si="3"/>
         <v>268255</v>
       </c>
-      <c r="E42" s="7" t="str">
+      <c r="E42" s="6" t="str">
         <f t="shared" si="4"/>
         <v>417DF</v>
       </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="9">
+      <c r="F42" s="7"/>
+      <c r="G42" s="8">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3643,16 +3640,16 @@
       <c r="C43" s="4">
         <v>25.6972</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="4">
         <f t="shared" si="3"/>
         <v>256972</v>
       </c>
-      <c r="E43" s="7" t="str">
+      <c r="E43" s="6" t="str">
         <f t="shared" si="4"/>
         <v>3EBCC</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="9">
+      <c r="F43" s="7"/>
+      <c r="G43" s="8">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
@@ -3661,16 +3658,16 @@
       <c r="C44" s="4">
         <v>24.629</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="4">
         <f t="shared" si="3"/>
         <v>246290</v>
       </c>
-      <c r="E44" s="7" t="str">
+      <c r="E44" s="6" t="str">
         <f t="shared" si="4"/>
         <v>3C212</v>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9">
+      <c r="F44" s="7"/>
+      <c r="G44" s="8">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
@@ -3679,16 +3676,16 @@
       <c r="C45" s="4">
         <v>23.6176</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="4">
         <f t="shared" si="3"/>
         <v>236176</v>
       </c>
-      <c r="E45" s="7" t="str">
+      <c r="E45" s="6" t="str">
         <f t="shared" si="4"/>
         <v>39A90</v>
       </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="9">
+      <c r="F45" s="7"/>
+      <c r="G45" s="8">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
@@ -3697,16 +3694,16 @@
       <c r="C46" s="4">
         <v>22.6597</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="4">
         <f t="shared" si="3"/>
         <v>226597</v>
       </c>
-      <c r="E46" s="7" t="str">
+      <c r="E46" s="6" t="str">
         <f t="shared" si="4"/>
         <v>37525</v>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="9">
+      <c r="F46" s="7"/>
+      <c r="G46" s="8">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
@@ -3715,16 +3712,16 @@
       <c r="C47" s="4">
         <v>21.7522</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="4">
         <f t="shared" si="3"/>
         <v>217522</v>
       </c>
-      <c r="E47" s="7" t="str">
+      <c r="E47" s="6" t="str">
         <f t="shared" si="4"/>
         <v>351B2</v>
       </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="9">
+      <c r="F47" s="7"/>
+      <c r="G47" s="8">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
@@ -3733,16 +3730,16 @@
       <c r="C48" s="4">
         <v>20.8916</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="4">
         <f t="shared" si="3"/>
         <v>208916</v>
       </c>
-      <c r="E48" s="7" t="str">
+      <c r="E48" s="6" t="str">
         <f t="shared" si="4"/>
         <v>33014</v>
       </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="9">
+      <c r="F48" s="7"/>
+      <c r="G48" s="8">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
@@ -3751,16 +3748,16 @@
       <c r="C49" s="4">
         <v>20.0749</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="4">
         <f t="shared" si="3"/>
         <v>200749</v>
       </c>
-      <c r="E49" s="7" t="str">
+      <c r="E49" s="6" t="str">
         <f t="shared" si="4"/>
         <v>3102D</v>
       </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="9">
+      <c r="F49" s="7"/>
+      <c r="G49" s="8">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
@@ -3769,16 +3766,16 @@
       <c r="C50" s="4">
         <v>19.2988</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D50" s="4">
         <f t="shared" si="3"/>
         <v>192988</v>
       </c>
-      <c r="E50" s="7" t="str">
+      <c r="E50" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2F1DC</v>
       </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="9">
+      <c r="F50" s="7"/>
+      <c r="G50" s="8">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
@@ -3787,16 +3784,16 @@
       <c r="C51" s="4">
         <v>18.56</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51" s="4">
         <f t="shared" si="3"/>
         <v>185600</v>
       </c>
-      <c r="E51" s="7" t="str">
+      <c r="E51" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2D500</v>
       </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="9">
+      <c r="F51" s="7"/>
+      <c r="G51" s="8">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
@@ -3805,34 +3802,34 @@
       <c r="C52" s="4">
         <v>18.4818</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="4">
         <f t="shared" si="3"/>
         <v>184818</v>
       </c>
-      <c r="E52" s="7" t="str">
+      <c r="E52" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2D1F2</v>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="9">
+      <c r="F52" s="7"/>
+      <c r="G52" s="8">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
     <row r="53" spans="3:7">
-      <c r="C53" s="6">
+      <c r="C53" s="5">
         <v>18.1489</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53" s="4">
         <f t="shared" si="3"/>
         <v>181489</v>
       </c>
-      <c r="E53" s="7" t="str">
+      <c r="E53" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2C4F1</v>
       </c>
-      <c r="F53" s="8"/>
-      <c r="G53" s="9">
+      <c r="F53" s="7"/>
+      <c r="G53" s="8">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
@@ -3841,16 +3838,16 @@
       <c r="C54" s="4">
         <v>17.6316</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54" s="4">
         <f t="shared" si="3"/>
         <v>176316</v>
       </c>
-      <c r="E54" s="7" t="str">
+      <c r="E54" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2B0BC</v>
       </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="9">
+      <c r="F54" s="7"/>
+      <c r="G54" s="8">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
@@ -3859,16 +3856,16 @@
       <c r="C55" s="4">
         <v>16.9917</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="4">
         <f t="shared" si="3"/>
         <v>169917</v>
       </c>
-      <c r="E55" s="7" t="str">
+      <c r="E55" s="6" t="str">
         <f t="shared" si="4"/>
         <v>297BD</v>
       </c>
-      <c r="F55" s="8"/>
-      <c r="G55" s="9">
+      <c r="F55" s="7"/>
+      <c r="G55" s="8">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
@@ -3877,16 +3874,16 @@
       <c r="C56" s="4">
         <v>16.2797</v>
       </c>
-      <c r="D56" s="5">
+      <c r="D56" s="4">
         <f t="shared" si="3"/>
         <v>162797</v>
       </c>
-      <c r="E56" s="7" t="str">
+      <c r="E56" s="6" t="str">
         <f t="shared" si="4"/>
         <v>27BED</v>
       </c>
-      <c r="F56" s="8"/>
-      <c r="G56" s="9">
+      <c r="F56" s="7"/>
+      <c r="G56" s="8">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
@@ -3895,16 +3892,16 @@
       <c r="C57" s="4">
         <v>15.535</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="4">
         <f t="shared" si="3"/>
         <v>155350</v>
       </c>
-      <c r="E57" s="7" t="str">
+      <c r="E57" s="6" t="str">
         <f t="shared" si="4"/>
         <v>25ED6</v>
       </c>
-      <c r="F57" s="8"/>
-      <c r="G57" s="9">
+      <c r="F57" s="7"/>
+      <c r="G57" s="8">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
@@ -3913,16 +3910,16 @@
       <c r="C58" s="4">
         <v>14.7867</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="4">
         <f t="shared" si="3"/>
         <v>147867</v>
       </c>
-      <c r="E58" s="7" t="str">
+      <c r="E58" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2419B</v>
       </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="9">
+      <c r="F58" s="7"/>
+      <c r="G58" s="8">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
@@ -3931,16 +3928,16 @@
       <c r="C59" s="4">
         <v>14.0551</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D59" s="4">
         <f t="shared" si="3"/>
         <v>140551</v>
       </c>
-      <c r="E59" s="7" t="str">
+      <c r="E59" s="6" t="str">
         <f t="shared" si="4"/>
         <v>22507</v>
       </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="9">
+      <c r="F59" s="7"/>
+      <c r="G59" s="8">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
@@ -3949,16 +3946,16 @@
       <c r="C60" s="4">
         <v>13.3536</v>
       </c>
-      <c r="D60" s="5">
+      <c r="D60" s="4">
         <f t="shared" si="3"/>
         <v>133536</v>
       </c>
-      <c r="E60" s="7" t="str">
+      <c r="E60" s="6" t="str">
         <f t="shared" si="4"/>
         <v>209A0</v>
       </c>
-      <c r="F60" s="8"/>
-      <c r="G60" s="9">
+      <c r="F60" s="7"/>
+      <c r="G60" s="8">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
@@ -3967,16 +3964,16 @@
       <c r="C61" s="4">
         <v>12.69</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61" s="4">
         <f t="shared" si="3"/>
         <v>126900</v>
       </c>
-      <c r="E61" s="7" t="str">
+      <c r="E61" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1EFB4</v>
       </c>
-      <c r="F61" s="8"/>
-      <c r="G61" s="9">
+      <c r="F61" s="7"/>
+      <c r="G61" s="8">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
@@ -3985,16 +3982,16 @@
       <c r="C62" s="4">
         <v>12.0684</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D62" s="4">
         <f t="shared" si="3"/>
         <v>120684</v>
       </c>
-      <c r="E62" s="7" t="str">
+      <c r="E62" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1D76C</v>
       </c>
-      <c r="F62" s="8"/>
-      <c r="G62" s="9">
+      <c r="F62" s="7"/>
+      <c r="G62" s="8">
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
@@ -4003,16 +4000,16 @@
       <c r="C63" s="4">
         <v>11.49</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D63" s="4">
         <f t="shared" si="3"/>
         <v>114900</v>
       </c>
-      <c r="E63" s="7" t="str">
+      <c r="E63" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1C0D4</v>
       </c>
-      <c r="F63" s="8"/>
-      <c r="G63" s="9">
+      <c r="F63" s="7"/>
+      <c r="G63" s="8">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
@@ -4021,16 +4018,16 @@
       <c r="C64" s="4">
         <v>10.9539</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64" s="4">
         <f t="shared" si="3"/>
         <v>109539</v>
       </c>
-      <c r="E64" s="7" t="str">
+      <c r="E64" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1ABE3</v>
       </c>
-      <c r="F64" s="8"/>
-      <c r="G64" s="9">
+      <c r="F64" s="7"/>
+      <c r="G64" s="8">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
@@ -4039,34 +4036,34 @@
       <c r="C65" s="4">
         <v>10.4582</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65" s="4">
         <f t="shared" si="3"/>
         <v>104582</v>
       </c>
-      <c r="E65" s="7" t="str">
+      <c r="E65" s="6" t="str">
         <f t="shared" si="4"/>
         <v>19886</v>
       </c>
-      <c r="F65" s="8"/>
-      <c r="G65" s="9">
+      <c r="F65" s="7"/>
+      <c r="G65" s="8">
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
     </row>
     <row r="66" spans="3:7">
-      <c r="C66" s="6">
+      <c r="C66" s="5">
         <v>10</v>
       </c>
-      <c r="D66" s="5">
+      <c r="D66" s="4">
         <f t="shared" ref="D66:D97" si="6">C66*10000</f>
         <v>100000</v>
       </c>
-      <c r="E66" s="7" t="str">
+      <c r="E66" s="6" t="str">
         <f t="shared" ref="E66:E97" si="7">DEC2HEX(D66)</f>
         <v>186A0</v>
       </c>
-      <c r="F66" s="8"/>
-      <c r="G66" s="9">
+      <c r="F66" s="7"/>
+      <c r="G66" s="8">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
@@ -4075,16 +4072,16 @@
       <c r="C67" s="4">
         <v>9.5762</v>
       </c>
-      <c r="D67" s="5">
+      <c r="D67" s="4">
         <f t="shared" si="6"/>
         <v>95762</v>
       </c>
-      <c r="E67" s="7" t="str">
+      <c r="E67" s="6" t="str">
         <f t="shared" si="7"/>
         <v>17612</v>
       </c>
-      <c r="F67" s="8"/>
-      <c r="G67" s="9">
+      <c r="F67" s="7"/>
+      <c r="G67" s="8">
         <f t="shared" ref="G67:G98" si="8">G66+1</f>
         <v>26</v>
       </c>
@@ -4093,16 +4090,16 @@
       <c r="C68" s="4">
         <v>9.1835</v>
       </c>
-      <c r="D68" s="5">
+      <c r="D68" s="4">
         <f t="shared" si="6"/>
         <v>91835</v>
       </c>
-      <c r="E68" s="7" t="str">
+      <c r="E68" s="6" t="str">
         <f t="shared" si="7"/>
         <v>166BB</v>
       </c>
-      <c r="F68" s="8"/>
-      <c r="G68" s="9">
+      <c r="F68" s="7"/>
+      <c r="G68" s="8">
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
@@ -4111,16 +4108,16 @@
       <c r="C69" s="4">
         <v>8.8186</v>
       </c>
-      <c r="D69" s="5">
+      <c r="D69" s="4">
         <f t="shared" si="6"/>
         <v>88186</v>
       </c>
-      <c r="E69" s="7" t="str">
+      <c r="E69" s="6" t="str">
         <f t="shared" si="7"/>
         <v>1587A</v>
       </c>
-      <c r="F69" s="8"/>
-      <c r="G69" s="9">
+      <c r="F69" s="7"/>
+      <c r="G69" s="8">
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
@@ -4129,16 +4126,16 @@
       <c r="C70" s="4">
         <v>8.4784</v>
       </c>
-      <c r="D70" s="5">
+      <c r="D70" s="4">
         <f t="shared" si="6"/>
         <v>84784</v>
       </c>
-      <c r="E70" s="7" t="str">
+      <c r="E70" s="6" t="str">
         <f t="shared" si="7"/>
         <v>14B30</v>
       </c>
-      <c r="F70" s="8"/>
-      <c r="G70" s="9">
+      <c r="F70" s="7"/>
+      <c r="G70" s="8">
         <f t="shared" si="8"/>
         <v>29</v>
       </c>
@@ -4147,16 +4144,16 @@
       <c r="C71" s="4">
         <v>8.16</v>
       </c>
-      <c r="D71" s="5">
+      <c r="D71" s="4">
         <f t="shared" si="6"/>
         <v>81600</v>
       </c>
-      <c r="E71" s="7" t="str">
+      <c r="E71" s="6" t="str">
         <f t="shared" si="7"/>
         <v>13EC0</v>
       </c>
-      <c r="F71" s="8"/>
-      <c r="G71" s="9">
+      <c r="F71" s="7"/>
+      <c r="G71" s="8">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
@@ -4165,16 +4162,16 @@
       <c r="C72" s="4">
         <v>7.8608</v>
       </c>
-      <c r="D72" s="5">
+      <c r="D72" s="4">
         <f t="shared" si="6"/>
         <v>78608</v>
       </c>
-      <c r="E72" s="7" t="str">
+      <c r="E72" s="6" t="str">
         <f t="shared" si="7"/>
         <v>13310</v>
       </c>
-      <c r="F72" s="8"/>
-      <c r="G72" s="9">
+      <c r="F72" s="7"/>
+      <c r="G72" s="8">
         <f t="shared" si="8"/>
         <v>31</v>
       </c>
@@ -4183,16 +4180,16 @@
       <c r="C73" s="4">
         <v>7.5785</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D73" s="4">
         <f t="shared" si="6"/>
         <v>75785</v>
       </c>
-      <c r="E73" s="7" t="str">
+      <c r="E73" s="6" t="str">
         <f t="shared" si="7"/>
         <v>12809</v>
       </c>
-      <c r="F73" s="8"/>
-      <c r="G73" s="9">
+      <c r="F73" s="7"/>
+      <c r="G73" s="8">
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
@@ -4201,16 +4198,16 @@
       <c r="C74" s="4">
         <v>7.3109</v>
       </c>
-      <c r="D74" s="5">
+      <c r="D74" s="4">
         <f t="shared" si="6"/>
         <v>73109</v>
       </c>
-      <c r="E74" s="7" t="str">
+      <c r="E74" s="6" t="str">
         <f t="shared" si="7"/>
         <v>11D95</v>
       </c>
-      <c r="F74" s="8"/>
-      <c r="G74" s="9">
+      <c r="F74" s="7"/>
+      <c r="G74" s="8">
         <f t="shared" si="8"/>
         <v>33</v>
       </c>
@@ -4219,16 +4216,16 @@
       <c r="C75" s="4">
         <v>7.0564</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="4">
         <f t="shared" si="6"/>
         <v>70564</v>
       </c>
-      <c r="E75" s="7" t="str">
+      <c r="E75" s="6" t="str">
         <f t="shared" si="7"/>
         <v>113A4</v>
       </c>
-      <c r="F75" s="8"/>
-      <c r="G75" s="9">
+      <c r="F75" s="7"/>
+      <c r="G75" s="8">
         <f t="shared" si="8"/>
         <v>34</v>
       </c>
@@ -4237,16 +4234,16 @@
       <c r="C76" s="4">
         <v>6.8133</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76" s="4">
         <f t="shared" si="6"/>
         <v>68133</v>
       </c>
-      <c r="E76" s="7" t="str">
+      <c r="E76" s="6" t="str">
         <f t="shared" si="7"/>
         <v>10A25</v>
       </c>
-      <c r="F76" s="8"/>
-      <c r="G76" s="9">
+      <c r="F76" s="7"/>
+      <c r="G76" s="8">
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
@@ -4255,16 +4252,16 @@
       <c r="C77" s="4">
         <v>6.5806</v>
       </c>
-      <c r="D77" s="5">
+      <c r="D77" s="4">
         <f t="shared" si="6"/>
         <v>65806</v>
       </c>
-      <c r="E77" s="7" t="str">
+      <c r="E77" s="6" t="str">
         <f t="shared" si="7"/>
         <v>1010E</v>
       </c>
-      <c r="F77" s="8"/>
-      <c r="G77" s="9">
+      <c r="F77" s="7"/>
+      <c r="G77" s="8">
         <f t="shared" si="8"/>
         <v>36</v>
       </c>
@@ -4273,34 +4270,34 @@
       <c r="C78" s="4">
         <v>6.357</v>
       </c>
-      <c r="D78" s="5">
+      <c r="D78" s="4">
         <f t="shared" si="6"/>
         <v>63570</v>
       </c>
-      <c r="E78" s="7" t="str">
+      <c r="E78" s="6" t="str">
         <f t="shared" si="7"/>
         <v>F852</v>
       </c>
-      <c r="F78" s="8"/>
-      <c r="G78" s="9">
+      <c r="F78" s="7"/>
+      <c r="G78" s="8">
         <f t="shared" si="8"/>
         <v>37</v>
       </c>
     </row>
     <row r="79" spans="3:7">
-      <c r="C79" s="6">
+      <c r="C79" s="5">
         <v>6.1418</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="4">
         <f t="shared" si="6"/>
         <v>61418</v>
       </c>
-      <c r="E79" s="7" t="str">
+      <c r="E79" s="6" t="str">
         <f t="shared" si="7"/>
         <v>EFEA</v>
       </c>
-      <c r="F79" s="8"/>
-      <c r="G79" s="9">
+      <c r="F79" s="7"/>
+      <c r="G79" s="8">
         <f t="shared" si="8"/>
         <v>38</v>
       </c>
@@ -4309,16 +4306,16 @@
       <c r="C80" s="4">
         <v>5.9343</v>
       </c>
-      <c r="D80" s="5">
+      <c r="D80" s="4">
         <f t="shared" si="6"/>
         <v>59343</v>
       </c>
-      <c r="E80" s="7" t="str">
+      <c r="E80" s="6" t="str">
         <f t="shared" si="7"/>
         <v>E7CF</v>
       </c>
-      <c r="F80" s="8"/>
-      <c r="G80" s="9">
+      <c r="F80" s="7"/>
+      <c r="G80" s="8">
         <f t="shared" si="8"/>
         <v>39</v>
       </c>
@@ -4327,16 +4324,16 @@
       <c r="C81" s="4">
         <v>5.734</v>
       </c>
-      <c r="D81" s="5">
+      <c r="D81" s="4">
         <f t="shared" si="6"/>
         <v>57340</v>
       </c>
-      <c r="E81" s="7" t="str">
+      <c r="E81" s="6" t="str">
         <f t="shared" si="7"/>
         <v>DFFC</v>
       </c>
-      <c r="F81" s="8"/>
-      <c r="G81" s="9">
+      <c r="F81" s="7"/>
+      <c r="G81" s="8">
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
@@ -4345,16 +4342,16 @@
       <c r="C82" s="4">
         <v>5.5405</v>
       </c>
-      <c r="D82" s="5">
+      <c r="D82" s="4">
         <f t="shared" si="6"/>
         <v>55405</v>
       </c>
-      <c r="E82" s="7" t="str">
+      <c r="E82" s="6" t="str">
         <f t="shared" si="7"/>
         <v>D86D</v>
       </c>
-      <c r="F82" s="8"/>
-      <c r="G82" s="9">
+      <c r="F82" s="7"/>
+      <c r="G82" s="8">
         <f t="shared" si="8"/>
         <v>41</v>
       </c>
@@ -4363,16 +4360,16 @@
       <c r="C83" s="4">
         <v>5.3534</v>
       </c>
-      <c r="D83" s="5">
+      <c r="D83" s="4">
         <f t="shared" si="6"/>
         <v>53534</v>
       </c>
-      <c r="E83" s="7" t="str">
+      <c r="E83" s="6" t="str">
         <f t="shared" si="7"/>
         <v>D11E</v>
       </c>
-      <c r="F83" s="8"/>
-      <c r="G83" s="9">
+      <c r="F83" s="7"/>
+      <c r="G83" s="8">
         <f t="shared" si="8"/>
         <v>42</v>
       </c>
@@ -4381,16 +4378,16 @@
       <c r="C84" s="4">
         <v>5.1725</v>
       </c>
-      <c r="D84" s="5">
+      <c r="D84" s="4">
         <f t="shared" si="6"/>
         <v>51725</v>
       </c>
-      <c r="E84" s="7" t="str">
+      <c r="E84" s="6" t="str">
         <f t="shared" si="7"/>
         <v>CA0D</v>
       </c>
-      <c r="F84" s="8"/>
-      <c r="G84" s="9">
+      <c r="F84" s="7"/>
+      <c r="G84" s="8">
         <f t="shared" si="8"/>
         <v>43</v>
       </c>
@@ -4399,16 +4396,16 @@
       <c r="C85" s="4">
         <v>4.9976</v>
       </c>
-      <c r="D85" s="5">
+      <c r="D85" s="4">
         <f t="shared" si="6"/>
         <v>49976</v>
       </c>
-      <c r="E85" s="7" t="str">
+      <c r="E85" s="6" t="str">
         <f t="shared" si="7"/>
         <v>C338</v>
       </c>
-      <c r="F85" s="8"/>
-      <c r="G85" s="9">
+      <c r="F85" s="7"/>
+      <c r="G85" s="8">
         <f t="shared" si="8"/>
         <v>44</v>
       </c>
@@ -4417,16 +4414,16 @@
       <c r="C86" s="4">
         <v>4.8286</v>
       </c>
-      <c r="D86" s="5">
+      <c r="D86" s="4">
         <f t="shared" si="6"/>
         <v>48286</v>
       </c>
-      <c r="E86" s="7" t="str">
+      <c r="E86" s="6" t="str">
         <f t="shared" si="7"/>
         <v>BC9E</v>
       </c>
-      <c r="F86" s="8"/>
-      <c r="G86" s="9">
+      <c r="F86" s="7"/>
+      <c r="G86" s="8">
         <f t="shared" si="8"/>
         <v>45</v>
       </c>
@@ -4435,16 +4432,16 @@
       <c r="C87" s="4">
         <v>4.6652</v>
       </c>
-      <c r="D87" s="5">
+      <c r="D87" s="4">
         <f t="shared" si="6"/>
         <v>46652</v>
       </c>
-      <c r="E87" s="7" t="str">
+      <c r="E87" s="6" t="str">
         <f t="shared" si="7"/>
         <v>B63C</v>
       </c>
-      <c r="F87" s="8"/>
-      <c r="G87" s="9">
+      <c r="F87" s="7"/>
+      <c r="G87" s="8">
         <f t="shared" si="8"/>
         <v>46</v>
       </c>
@@ -4453,16 +4450,16 @@
       <c r="C88" s="4">
         <v>4.5073</v>
       </c>
-      <c r="D88" s="5">
+      <c r="D88" s="4">
         <f t="shared" si="6"/>
         <v>45073</v>
       </c>
-      <c r="E88" s="7" t="str">
+      <c r="E88" s="6" t="str">
         <f t="shared" si="7"/>
         <v>B011</v>
       </c>
-      <c r="F88" s="8"/>
-      <c r="G88" s="9">
+      <c r="F88" s="7"/>
+      <c r="G88" s="8">
         <f t="shared" si="8"/>
         <v>47</v>
       </c>
@@ -4471,16 +4468,16 @@
       <c r="C89" s="4">
         <v>4.3548</v>
       </c>
-      <c r="D89" s="5">
+      <c r="D89" s="4">
         <f t="shared" si="6"/>
         <v>43548</v>
       </c>
-      <c r="E89" s="7" t="str">
+      <c r="E89" s="6" t="str">
         <f t="shared" si="7"/>
         <v>AA1C</v>
       </c>
-      <c r="F89" s="8"/>
-      <c r="G89" s="9">
+      <c r="F89" s="7"/>
+      <c r="G89" s="8">
         <f t="shared" si="8"/>
         <v>48</v>
       </c>
@@ -4489,16 +4486,16 @@
       <c r="C90" s="4">
         <v>4.2075</v>
       </c>
-      <c r="D90" s="5">
+      <c r="D90" s="4">
         <f t="shared" si="6"/>
         <v>42075</v>
       </c>
-      <c r="E90" s="7" t="str">
+      <c r="E90" s="6" t="str">
         <f t="shared" si="7"/>
         <v>A45B</v>
       </c>
-      <c r="F90" s="8"/>
-      <c r="G90" s="9">
+      <c r="F90" s="7"/>
+      <c r="G90" s="8">
         <f t="shared" si="8"/>
         <v>49</v>
       </c>
@@ -4507,34 +4504,34 @@
       <c r="C91" s="4">
         <v>4.065</v>
       </c>
-      <c r="D91" s="5">
+      <c r="D91" s="4">
         <f t="shared" si="6"/>
         <v>40650</v>
       </c>
-      <c r="E91" s="7" t="str">
+      <c r="E91" s="6" t="str">
         <f t="shared" si="7"/>
         <v>9ECA</v>
       </c>
-      <c r="F91" s="8"/>
-      <c r="G91" s="9">
+      <c r="F91" s="7"/>
+      <c r="G91" s="8">
         <f t="shared" si="8"/>
         <v>50</v>
       </c>
     </row>
     <row r="92" spans="3:7">
-      <c r="C92" s="6">
+      <c r="C92" s="5">
         <v>3.9271</v>
       </c>
-      <c r="D92" s="5">
+      <c r="D92" s="4">
         <f t="shared" si="6"/>
         <v>39271</v>
       </c>
-      <c r="E92" s="7" t="str">
+      <c r="E92" s="6" t="str">
         <f t="shared" si="7"/>
         <v>9967</v>
       </c>
-      <c r="F92" s="8"/>
-      <c r="G92" s="9">
+      <c r="F92" s="7"/>
+      <c r="G92" s="8">
         <f t="shared" si="8"/>
         <v>51</v>
       </c>
@@ -4543,16 +4540,16 @@
       <c r="C93" s="4">
         <v>3.7936</v>
       </c>
-      <c r="D93" s="5">
+      <c r="D93" s="4">
         <f t="shared" si="6"/>
         <v>37936</v>
       </c>
-      <c r="E93" s="7" t="str">
+      <c r="E93" s="6" t="str">
         <f t="shared" si="7"/>
         <v>9430</v>
       </c>
-      <c r="F93" s="8"/>
-      <c r="G93" s="9">
+      <c r="F93" s="7"/>
+      <c r="G93" s="8">
         <f t="shared" si="8"/>
         <v>52</v>
       </c>
@@ -4561,16 +4558,16 @@
       <c r="C94" s="4">
         <v>3.6639</v>
       </c>
-      <c r="D94" s="5">
+      <c r="D94" s="4">
         <f t="shared" si="6"/>
         <v>36639</v>
       </c>
-      <c r="E94" s="7" t="str">
+      <c r="E94" s="6" t="str">
         <f t="shared" si="7"/>
         <v>8F1F</v>
       </c>
-      <c r="F94" s="8"/>
-      <c r="G94" s="9">
+      <c r="F94" s="7"/>
+      <c r="G94" s="8">
         <f t="shared" si="8"/>
         <v>53</v>
       </c>
@@ -4579,16 +4576,16 @@
       <c r="C95" s="4">
         <v>3.5377</v>
       </c>
-      <c r="D95" s="5">
+      <c r="D95" s="4">
         <f t="shared" si="6"/>
         <v>35377</v>
       </c>
-      <c r="E95" s="7" t="str">
+      <c r="E95" s="6" t="str">
         <f t="shared" si="7"/>
         <v>8A31</v>
       </c>
-      <c r="F95" s="8"/>
-      <c r="G95" s="9">
+      <c r="F95" s="7"/>
+      <c r="G95" s="8">
         <f t="shared" si="8"/>
         <v>54</v>
       </c>
@@ -4597,16 +4594,16 @@
       <c r="C96" s="4">
         <v>3.4146</v>
       </c>
-      <c r="D96" s="5">
+      <c r="D96" s="4">
         <f t="shared" si="6"/>
         <v>34146</v>
       </c>
-      <c r="E96" s="7" t="str">
+      <c r="E96" s="6" t="str">
         <f t="shared" si="7"/>
         <v>8562</v>
       </c>
-      <c r="F96" s="8"/>
-      <c r="G96" s="9">
+      <c r="F96" s="7"/>
+      <c r="G96" s="8">
         <f t="shared" si="8"/>
         <v>55</v>
       </c>
@@ -4615,16 +4612,16 @@
       <c r="C97" s="4">
         <v>3.2939</v>
       </c>
-      <c r="D97" s="5">
+      <c r="D97" s="4">
         <f t="shared" si="6"/>
         <v>32939</v>
       </c>
-      <c r="E97" s="7" t="str">
+      <c r="E97" s="6" t="str">
         <f t="shared" si="7"/>
         <v>80AB</v>
       </c>
-      <c r="F97" s="8"/>
-      <c r="G97" s="9">
+      <c r="F97" s="7"/>
+      <c r="G97" s="8">
         <f t="shared" si="8"/>
         <v>56</v>
       </c>
@@ -4633,16 +4630,16 @@
       <c r="C98" s="4">
         <v>3.1752</v>
       </c>
-      <c r="D98" s="5">
+      <c r="D98" s="4">
         <f t="shared" ref="D98:D129" si="9">C98*10000</f>
         <v>31752</v>
       </c>
-      <c r="E98" s="7" t="str">
+      <c r="E98" s="6" t="str">
         <f t="shared" ref="E98:E129" si="10">DEC2HEX(D98)</f>
         <v>7C08</v>
       </c>
-      <c r="F98" s="8"/>
-      <c r="G98" s="9">
+      <c r="F98" s="7"/>
+      <c r="G98" s="8">
         <f t="shared" si="8"/>
         <v>57</v>
       </c>
@@ -4651,16 +4648,16 @@
       <c r="C99" s="4">
         <v>3.0579</v>
       </c>
-      <c r="D99" s="5">
+      <c r="D99" s="4">
         <f t="shared" si="9"/>
         <v>30579</v>
       </c>
-      <c r="E99" s="7" t="str">
+      <c r="E99" s="6" t="str">
         <f t="shared" si="10"/>
         <v>7773</v>
       </c>
-      <c r="F99" s="8"/>
-      <c r="G99" s="9">
+      <c r="F99" s="7"/>
+      <c r="G99" s="8">
         <f t="shared" ref="G99:G130" si="11">G98+1</f>
         <v>58</v>
       </c>
@@ -4669,16 +4666,16 @@
       <c r="C100" s="4">
         <v>2.9414</v>
       </c>
-      <c r="D100" s="5">
+      <c r="D100" s="4">
         <f t="shared" si="9"/>
         <v>29414</v>
       </c>
-      <c r="E100" s="7" t="str">
+      <c r="E100" s="6" t="str">
         <f t="shared" si="10"/>
         <v>72E6</v>
       </c>
-      <c r="F100" s="8"/>
-      <c r="G100" s="9">
+      <c r="F100" s="7"/>
+      <c r="G100" s="8">
         <f t="shared" si="11"/>
         <v>59</v>
       </c>
@@ -4687,16 +4684,16 @@
       <c r="C101" s="4">
         <v>2.825</v>
       </c>
-      <c r="D101" s="5">
+      <c r="D101" s="4">
         <f t="shared" si="9"/>
         <v>28250</v>
       </c>
-      <c r="E101" s="7" t="str">
+      <c r="E101" s="6" t="str">
         <f t="shared" si="10"/>
         <v>6E5A</v>
       </c>
-      <c r="F101" s="8"/>
-      <c r="G101" s="9">
+      <c r="F101" s="7"/>
+      <c r="G101" s="8">
         <f t="shared" si="11"/>
         <v>60</v>
       </c>
@@ -4705,16 +4702,16 @@
       <c r="C102" s="4">
         <v>2.7762</v>
       </c>
-      <c r="D102" s="5">
+      <c r="D102" s="4">
         <f t="shared" si="9"/>
         <v>27762</v>
       </c>
-      <c r="E102" s="7" t="str">
+      <c r="E102" s="6" t="str">
         <f t="shared" si="10"/>
         <v>6C72</v>
       </c>
-      <c r="F102" s="8"/>
-      <c r="G102" s="9">
+      <c r="F102" s="7"/>
+      <c r="G102" s="8">
         <f t="shared" si="11"/>
         <v>61</v>
       </c>
@@ -4723,16 +4720,16 @@
       <c r="C103" s="4">
         <v>2.7179</v>
       </c>
-      <c r="D103" s="5">
+      <c r="D103" s="4">
         <f t="shared" si="9"/>
         <v>27179</v>
       </c>
-      <c r="E103" s="7" t="str">
+      <c r="E103" s="6" t="str">
         <f t="shared" si="10"/>
         <v>6A2B</v>
       </c>
-      <c r="F103" s="8"/>
-      <c r="G103" s="9">
+      <c r="F103" s="7"/>
+      <c r="G103" s="8">
         <f t="shared" si="11"/>
         <v>62</v>
       </c>
@@ -4741,34 +4738,34 @@
       <c r="C104" s="4">
         <v>2.6523</v>
       </c>
-      <c r="D104" s="5">
+      <c r="D104" s="4">
         <f t="shared" si="9"/>
         <v>26523</v>
       </c>
-      <c r="E104" s="7" t="str">
+      <c r="E104" s="6" t="str">
         <f t="shared" si="10"/>
         <v>679B</v>
       </c>
-      <c r="F104" s="8"/>
-      <c r="G104" s="9">
+      <c r="F104" s="7"/>
+      <c r="G104" s="8">
         <f t="shared" si="11"/>
         <v>63</v>
       </c>
     </row>
     <row r="105" spans="3:7">
-      <c r="C105" s="6">
+      <c r="C105" s="5">
         <v>2.5817</v>
       </c>
-      <c r="D105" s="5">
+      <c r="D105" s="4">
         <f t="shared" si="9"/>
         <v>25817</v>
       </c>
-      <c r="E105" s="7" t="str">
+      <c r="E105" s="6" t="str">
         <f t="shared" si="10"/>
         <v>64D9</v>
       </c>
-      <c r="F105" s="8"/>
-      <c r="G105" s="9">
+      <c r="F105" s="7"/>
+      <c r="G105" s="8">
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
@@ -4777,16 +4774,16 @@
       <c r="C106" s="4">
         <v>2.5076</v>
       </c>
-      <c r="D106" s="5">
+      <c r="D106" s="4">
         <f t="shared" si="9"/>
         <v>25076</v>
       </c>
-      <c r="E106" s="7" t="str">
+      <c r="E106" s="6" t="str">
         <f t="shared" si="10"/>
         <v>61F4</v>
       </c>
-      <c r="F106" s="8"/>
-      <c r="G106" s="9">
+      <c r="F106" s="7"/>
+      <c r="G106" s="8">
         <f t="shared" si="11"/>
         <v>65</v>
       </c>
@@ -4795,16 +4792,16 @@
       <c r="C107" s="4">
         <v>2.4319</v>
       </c>
-      <c r="D107" s="5">
+      <c r="D107" s="4">
         <f t="shared" si="9"/>
         <v>24319</v>
       </c>
-      <c r="E107" s="7" t="str">
+      <c r="E107" s="6" t="str">
         <f t="shared" si="10"/>
         <v>5EFF</v>
       </c>
-      <c r="F107" s="8"/>
-      <c r="G107" s="9">
+      <c r="F107" s="7"/>
+      <c r="G107" s="8">
         <f t="shared" si="11"/>
         <v>66</v>
       </c>
@@ -4813,16 +4810,16 @@
       <c r="C108" s="4">
         <v>2.3557</v>
       </c>
-      <c r="D108" s="5">
+      <c r="D108" s="4">
         <f t="shared" si="9"/>
         <v>23557</v>
       </c>
-      <c r="E108" s="7" t="str">
+      <c r="E108" s="6" t="str">
         <f t="shared" si="10"/>
         <v>5C05</v>
       </c>
-      <c r="F108" s="8"/>
-      <c r="G108" s="9">
+      <c r="F108" s="7"/>
+      <c r="G108" s="8">
         <f t="shared" si="11"/>
         <v>67</v>
       </c>
@@ -4831,16 +4828,16 @@
       <c r="C109" s="4">
         <v>2.2803</v>
       </c>
-      <c r="D109" s="5">
+      <c r="D109" s="4">
         <f t="shared" si="9"/>
         <v>22803</v>
       </c>
-      <c r="E109" s="7" t="str">
+      <c r="E109" s="6" t="str">
         <f t="shared" si="10"/>
         <v>5913</v>
       </c>
-      <c r="F109" s="8"/>
-      <c r="G109" s="9">
+      <c r="F109" s="7"/>
+      <c r="G109" s="8">
         <f t="shared" si="11"/>
         <v>68</v>
       </c>
@@ -4849,34 +4846,34 @@
       <c r="C110" s="4">
         <v>2.2065</v>
       </c>
-      <c r="D110" s="5">
+      <c r="D110" s="4">
         <f t="shared" si="9"/>
         <v>22065</v>
       </c>
-      <c r="E110" s="7" t="str">
+      <c r="E110" s="6" t="str">
         <f t="shared" si="10"/>
         <v>5631</v>
       </c>
-      <c r="F110" s="8"/>
-      <c r="G110" s="9">
+      <c r="F110" s="7"/>
+      <c r="G110" s="8">
         <f t="shared" si="11"/>
         <v>69</v>
       </c>
     </row>
     <row r="111" spans="3:7">
-      <c r="C111" s="6">
+      <c r="C111" s="5">
         <v>2.135</v>
       </c>
-      <c r="D111" s="5">
+      <c r="D111" s="4">
         <f t="shared" si="9"/>
         <v>21350</v>
       </c>
-      <c r="E111" s="7" t="str">
+      <c r="E111" s="6" t="str">
         <f t="shared" si="10"/>
         <v>5366</v>
       </c>
-      <c r="F111" s="8"/>
-      <c r="G111" s="9">
+      <c r="F111" s="7"/>
+      <c r="G111" s="8">
         <f t="shared" si="11"/>
         <v>70</v>
       </c>
@@ -4885,16 +4882,16 @@
       <c r="C112" s="4">
         <v>2.0661</v>
       </c>
-      <c r="D112" s="5">
+      <c r="D112" s="4">
         <f t="shared" si="9"/>
         <v>20661</v>
       </c>
-      <c r="E112" s="7" t="str">
+      <c r="E112" s="6" t="str">
         <f t="shared" si="10"/>
         <v>50B5</v>
       </c>
-      <c r="F112" s="8"/>
-      <c r="G112" s="9">
+      <c r="F112" s="7"/>
+      <c r="G112" s="8">
         <f t="shared" si="11"/>
         <v>71</v>
       </c>
@@ -4903,16 +4900,16 @@
       <c r="C113" s="4">
         <v>2.0004</v>
       </c>
-      <c r="D113" s="5">
+      <c r="D113" s="4">
         <f t="shared" si="9"/>
         <v>20004</v>
       </c>
-      <c r="E113" s="7" t="str">
+      <c r="E113" s="6" t="str">
         <f t="shared" si="10"/>
         <v>4E24</v>
       </c>
-      <c r="F113" s="8"/>
-      <c r="G113" s="9">
+      <c r="F113" s="7"/>
+      <c r="G113" s="8">
         <f t="shared" si="11"/>
         <v>72</v>
       </c>
@@ -4921,16 +4918,16 @@
       <c r="C114" s="4">
         <v>1.9378</v>
       </c>
-      <c r="D114" s="5">
+      <c r="D114" s="4">
         <f t="shared" si="9"/>
         <v>19378</v>
       </c>
-      <c r="E114" s="7" t="str">
+      <c r="E114" s="6" t="str">
         <f t="shared" si="10"/>
         <v>4BB2</v>
       </c>
-      <c r="F114" s="8"/>
-      <c r="G114" s="9">
+      <c r="F114" s="7"/>
+      <c r="G114" s="8">
         <f t="shared" si="11"/>
         <v>73</v>
       </c>
@@ -4939,16 +4936,16 @@
       <c r="C115" s="4">
         <v>1.8785</v>
       </c>
-      <c r="D115" s="5">
+      <c r="D115" s="4">
         <f t="shared" si="9"/>
         <v>18785</v>
       </c>
-      <c r="E115" s="7" t="str">
+      <c r="E115" s="6" t="str">
         <f t="shared" si="10"/>
         <v>4961</v>
       </c>
-      <c r="F115" s="8"/>
-      <c r="G115" s="9">
+      <c r="F115" s="7"/>
+      <c r="G115" s="8">
         <f t="shared" si="11"/>
         <v>74</v>
       </c>
@@ -4957,16 +4954,16 @@
       <c r="C116" s="4">
         <v>1.8225</v>
       </c>
-      <c r="D116" s="5">
+      <c r="D116" s="4">
         <f t="shared" si="9"/>
         <v>18225</v>
       </c>
-      <c r="E116" s="7" t="str">
+      <c r="E116" s="6" t="str">
         <f t="shared" si="10"/>
         <v>4731</v>
       </c>
-      <c r="F116" s="8"/>
-      <c r="G116" s="9">
+      <c r="F116" s="7"/>
+      <c r="G116" s="8">
         <f t="shared" si="11"/>
         <v>75</v>
       </c>
@@ -4975,34 +4972,34 @@
       <c r="C117" s="4">
         <v>1.7696</v>
       </c>
-      <c r="D117" s="5">
+      <c r="D117" s="4">
         <f t="shared" si="9"/>
         <v>17696</v>
       </c>
-      <c r="E117" s="7" t="str">
+      <c r="E117" s="6" t="str">
         <f t="shared" si="10"/>
         <v>4520</v>
       </c>
-      <c r="F117" s="8"/>
-      <c r="G117" s="9">
+      <c r="F117" s="7"/>
+      <c r="G117" s="8">
         <f t="shared" si="11"/>
         <v>76</v>
       </c>
     </row>
     <row r="118" spans="3:7">
-      <c r="C118" s="6">
+      <c r="C118" s="5">
         <v>1.7197</v>
       </c>
-      <c r="D118" s="5">
+      <c r="D118" s="4">
         <f t="shared" si="9"/>
         <v>17197</v>
       </c>
-      <c r="E118" s="7" t="str">
+      <c r="E118" s="6" t="str">
         <f t="shared" si="10"/>
         <v>432D</v>
       </c>
-      <c r="F118" s="8"/>
-      <c r="G118" s="9">
+      <c r="F118" s="7"/>
+      <c r="G118" s="8">
         <f t="shared" si="11"/>
         <v>77</v>
       </c>
@@ -5011,16 +5008,16 @@
       <c r="C119" s="4">
         <v>1.6727</v>
       </c>
-      <c r="D119" s="5">
+      <c r="D119" s="4">
         <f t="shared" si="9"/>
         <v>16727</v>
       </c>
-      <c r="E119" s="7" t="str">
+      <c r="E119" s="6" t="str">
         <f t="shared" si="10"/>
         <v>4157</v>
       </c>
-      <c r="F119" s="8"/>
-      <c r="G119" s="9">
+      <c r="F119" s="7"/>
+      <c r="G119" s="8">
         <f t="shared" si="11"/>
         <v>78</v>
       </c>
@@ -5029,16 +5026,16 @@
       <c r="C120" s="4">
         <v>1.6282</v>
       </c>
-      <c r="D120" s="5">
+      <c r="D120" s="4">
         <f t="shared" si="9"/>
         <v>16282</v>
       </c>
-      <c r="E120" s="7" t="str">
+      <c r="E120" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3F9A</v>
       </c>
-      <c r="F120" s="8"/>
-      <c r="G120" s="9">
+      <c r="F120" s="7"/>
+      <c r="G120" s="8">
         <f t="shared" si="11"/>
         <v>79</v>
       </c>
@@ -5047,16 +5044,16 @@
       <c r="C121" s="4">
         <v>1.586</v>
       </c>
-      <c r="D121" s="5">
+      <c r="D121" s="4">
         <f t="shared" si="9"/>
         <v>15860</v>
       </c>
-      <c r="E121" s="7" t="str">
+      <c r="E121" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3DF4</v>
       </c>
-      <c r="F121" s="8"/>
-      <c r="G121" s="9">
+      <c r="F121" s="7"/>
+      <c r="G121" s="8">
         <f t="shared" si="11"/>
         <v>80</v>
       </c>
@@ -5065,16 +5062,16 @@
       <c r="C122" s="4">
         <v>1.5458</v>
       </c>
-      <c r="D122" s="5">
+      <c r="D122" s="4">
         <f t="shared" si="9"/>
         <v>15458</v>
       </c>
-      <c r="E122" s="7" t="str">
+      <c r="E122" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3C62</v>
       </c>
-      <c r="F122" s="8"/>
-      <c r="G122" s="9">
+      <c r="F122" s="7"/>
+      <c r="G122" s="8">
         <f t="shared" si="11"/>
         <v>81</v>
       </c>
@@ -5083,34 +5080,34 @@
       <c r="C123" s="4">
         <v>1.5075</v>
       </c>
-      <c r="D123" s="5">
+      <c r="D123" s="4">
         <f t="shared" si="9"/>
         <v>15075</v>
       </c>
-      <c r="E123" s="7" t="str">
+      <c r="E123" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3AE3</v>
       </c>
-      <c r="F123" s="8"/>
-      <c r="G123" s="9">
+      <c r="F123" s="7"/>
+      <c r="G123" s="8">
         <f t="shared" si="11"/>
         <v>82</v>
       </c>
     </row>
     <row r="124" spans="3:7">
-      <c r="C124" s="6">
+      <c r="C124" s="5">
         <v>1.4707</v>
       </c>
-      <c r="D124" s="5">
+      <c r="D124" s="4">
         <f t="shared" si="9"/>
         <v>14707</v>
       </c>
-      <c r="E124" s="7" t="str">
+      <c r="E124" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3973</v>
       </c>
-      <c r="F124" s="8"/>
-      <c r="G124" s="9">
+      <c r="F124" s="7"/>
+      <c r="G124" s="8">
         <f t="shared" si="11"/>
         <v>83</v>
       </c>
@@ -5119,16 +5116,16 @@
       <c r="C125" s="4">
         <v>1.4352</v>
       </c>
-      <c r="D125" s="5">
+      <c r="D125" s="4">
         <f t="shared" si="9"/>
         <v>14352</v>
       </c>
-      <c r="E125" s="7" t="str">
+      <c r="E125" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3810</v>
       </c>
-      <c r="F125" s="8"/>
-      <c r="G125" s="9">
+      <c r="F125" s="7"/>
+      <c r="G125" s="8">
         <f t="shared" si="11"/>
         <v>84</v>
       </c>
@@ -5137,16 +5134,16 @@
       <c r="C126" s="4">
         <v>1.4006</v>
       </c>
-      <c r="D126" s="5">
+      <c r="D126" s="4">
         <f t="shared" si="9"/>
         <v>14006</v>
       </c>
-      <c r="E126" s="7" t="str">
+      <c r="E126" s="6" t="str">
         <f t="shared" si="10"/>
         <v>36B6</v>
       </c>
-      <c r="F126" s="8"/>
-      <c r="G126" s="9">
+      <c r="F126" s="7"/>
+      <c r="G126" s="8">
         <f t="shared" si="11"/>
         <v>85</v>
       </c>
@@ -5155,16 +5152,16 @@
       <c r="C127" s="4">
         <v>1.3669</v>
       </c>
-      <c r="D127" s="5">
+      <c r="D127" s="4">
         <f t="shared" si="9"/>
         <v>13669</v>
       </c>
-      <c r="E127" s="7" t="str">
+      <c r="E127" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3565</v>
       </c>
-      <c r="F127" s="8"/>
-      <c r="G127" s="9">
+      <c r="F127" s="7"/>
+      <c r="G127" s="8">
         <f t="shared" si="11"/>
         <v>86</v>
       </c>
@@ -5173,16 +5170,16 @@
       <c r="C128" s="4">
         <v>1.3337</v>
       </c>
-      <c r="D128" s="5">
+      <c r="D128" s="4">
         <f t="shared" si="9"/>
         <v>13337</v>
       </c>
-      <c r="E128" s="7" t="str">
+      <c r="E128" s="6" t="str">
         <f t="shared" si="10"/>
         <v>3419</v>
       </c>
-      <c r="F128" s="8"/>
-      <c r="G128" s="9">
+      <c r="F128" s="7"/>
+      <c r="G128" s="8">
         <f t="shared" si="11"/>
         <v>87</v>
       </c>
@@ -5191,16 +5188,16 @@
       <c r="C129" s="4">
         <v>1.3009</v>
       </c>
-      <c r="D129" s="5">
+      <c r="D129" s="4">
         <f t="shared" si="9"/>
         <v>13009</v>
       </c>
-      <c r="E129" s="7" t="str">
+      <c r="E129" s="6" t="str">
         <f t="shared" si="10"/>
         <v>32D1</v>
       </c>
-      <c r="F129" s="8"/>
-      <c r="G129" s="9">
+      <c r="F129" s="7"/>
+      <c r="G129" s="8">
         <f t="shared" si="11"/>
         <v>88</v>
       </c>
@@ -5209,34 +5206,34 @@
       <c r="C130" s="4">
         <v>1.2684</v>
       </c>
-      <c r="D130" s="5">
+      <c r="D130" s="4">
         <f t="shared" ref="D130:D150" si="12">C130*10000</f>
         <v>12684</v>
       </c>
-      <c r="E130" s="7" t="str">
+      <c r="E130" s="6" t="str">
         <f t="shared" ref="E130:E150" si="13">DEC2HEX(D130)</f>
         <v>318C</v>
       </c>
-      <c r="F130" s="8"/>
-      <c r="G130" s="9">
+      <c r="F130" s="7"/>
+      <c r="G130" s="8">
         <f t="shared" si="11"/>
         <v>89</v>
       </c>
     </row>
     <row r="131" spans="3:7">
-      <c r="C131" s="6">
+      <c r="C131" s="5">
         <v>1.236</v>
       </c>
-      <c r="D131" s="5">
+      <c r="D131" s="4">
         <f t="shared" si="12"/>
         <v>12360</v>
       </c>
-      <c r="E131" s="7" t="str">
+      <c r="E131" s="6" t="str">
         <f t="shared" si="13"/>
         <v>3048</v>
       </c>
-      <c r="F131" s="8"/>
-      <c r="G131" s="9">
+      <c r="F131" s="7"/>
+      <c r="G131" s="8">
         <f t="shared" ref="G131:G150" si="14">G130+1</f>
         <v>90</v>
       </c>
@@ -5245,16 +5242,16 @@
       <c r="C132" s="4">
         <v>1.2037</v>
       </c>
-      <c r="D132" s="5">
+      <c r="D132" s="4">
         <f t="shared" si="12"/>
         <v>12037</v>
       </c>
-      <c r="E132" s="7" t="str">
+      <c r="E132" s="6" t="str">
         <f t="shared" si="13"/>
         <v>2F05</v>
       </c>
-      <c r="F132" s="8"/>
-      <c r="G132" s="9">
+      <c r="F132" s="7"/>
+      <c r="G132" s="8">
         <f t="shared" si="14"/>
         <v>91</v>
       </c>
@@ -5263,16 +5260,16 @@
       <c r="C133" s="4">
         <v>1.1714</v>
       </c>
-      <c r="D133" s="5">
+      <c r="D133" s="4">
         <f t="shared" si="12"/>
         <v>11714</v>
       </c>
-      <c r="E133" s="7" t="str">
+      <c r="E133" s="6" t="str">
         <f t="shared" si="13"/>
         <v>2DC2</v>
       </c>
-      <c r="F133" s="8"/>
-      <c r="G133" s="9">
+      <c r="F133" s="7"/>
+      <c r="G133" s="8">
         <f t="shared" si="14"/>
         <v>92</v>
       </c>
@@ -5281,16 +5278,16 @@
       <c r="C134" s="4">
         <v>1.139</v>
       </c>
-      <c r="D134" s="5">
+      <c r="D134" s="4">
         <f t="shared" si="12"/>
         <v>11390</v>
       </c>
-      <c r="E134" s="7" t="str">
+      <c r="E134" s="6" t="str">
         <f t="shared" si="13"/>
         <v>2C7E</v>
       </c>
-      <c r="F134" s="8"/>
-      <c r="G134" s="9">
+      <c r="F134" s="7"/>
+      <c r="G134" s="8">
         <f t="shared" si="14"/>
         <v>93</v>
       </c>
@@ -5299,16 +5296,16 @@
       <c r="C135" s="4">
         <v>1.1067</v>
       </c>
-      <c r="D135" s="5">
+      <c r="D135" s="4">
         <f t="shared" si="12"/>
         <v>11067</v>
       </c>
-      <c r="E135" s="7" t="str">
+      <c r="E135" s="6" t="str">
         <f t="shared" si="13"/>
         <v>2B3B</v>
       </c>
-      <c r="F135" s="8"/>
-      <c r="G135" s="9">
+      <c r="F135" s="7"/>
+      <c r="G135" s="8">
         <f t="shared" si="14"/>
         <v>94</v>
       </c>
@@ -5317,34 +5314,34 @@
       <c r="C136" s="4">
         <v>1.0744</v>
       </c>
-      <c r="D136" s="5">
+      <c r="D136" s="4">
         <f t="shared" si="12"/>
         <v>10744</v>
       </c>
-      <c r="E136" s="7" t="str">
+      <c r="E136" s="6" t="str">
         <f t="shared" si="13"/>
         <v>29F8</v>
       </c>
-      <c r="F136" s="8"/>
-      <c r="G136" s="9">
+      <c r="F136" s="7"/>
+      <c r="G136" s="8">
         <f t="shared" si="14"/>
         <v>95</v>
       </c>
     </row>
     <row r="137" spans="3:7">
-      <c r="C137" s="6">
+      <c r="C137" s="5">
         <v>1.0422</v>
       </c>
-      <c r="D137" s="5">
+      <c r="D137" s="4">
         <f t="shared" si="12"/>
         <v>10422</v>
       </c>
-      <c r="E137" s="7" t="str">
+      <c r="E137" s="6" t="str">
         <f t="shared" si="13"/>
         <v>28B6</v>
       </c>
-      <c r="F137" s="8"/>
-      <c r="G137" s="9">
+      <c r="F137" s="7"/>
+      <c r="G137" s="8">
         <f t="shared" si="14"/>
         <v>96</v>
       </c>
@@ -5353,16 +5350,16 @@
       <c r="C138" s="4">
         <v>1.0104</v>
       </c>
-      <c r="D138" s="5">
+      <c r="D138" s="4">
         <f t="shared" si="12"/>
         <v>10104</v>
       </c>
-      <c r="E138" s="7" t="str">
+      <c r="E138" s="6" t="str">
         <f t="shared" si="13"/>
         <v>2778</v>
       </c>
-      <c r="F138" s="8"/>
-      <c r="G138" s="9">
+      <c r="F138" s="7"/>
+      <c r="G138" s="8">
         <f t="shared" si="14"/>
         <v>97</v>
       </c>
@@ -5371,16 +5368,16 @@
       <c r="C139" s="4">
         <v>0.9789</v>
       </c>
-      <c r="D139" s="5">
+      <c r="D139" s="4">
         <f t="shared" si="12"/>
         <v>9789</v>
       </c>
-      <c r="E139" s="7" t="str">
+      <c r="E139" s="6" t="str">
         <f t="shared" si="13"/>
         <v>263D</v>
       </c>
-      <c r="F139" s="8"/>
-      <c r="G139" s="9">
+      <c r="F139" s="7"/>
+      <c r="G139" s="8">
         <f t="shared" si="14"/>
         <v>98</v>
       </c>
@@ -5389,16 +5386,16 @@
       <c r="C140" s="4">
         <v>0.9481</v>
       </c>
-      <c r="D140" s="5">
+      <c r="D140" s="4">
         <f t="shared" si="12"/>
         <v>9481</v>
       </c>
-      <c r="E140" s="7" t="str">
+      <c r="E140" s="6" t="str">
         <f t="shared" si="13"/>
         <v>2509</v>
       </c>
-      <c r="F140" s="8"/>
-      <c r="G140" s="9">
+      <c r="F140" s="7"/>
+      <c r="G140" s="8">
         <f t="shared" si="14"/>
         <v>99</v>
       </c>
@@ -5407,16 +5404,16 @@
       <c r="C141" s="4">
         <v>0.918</v>
       </c>
-      <c r="D141" s="5">
+      <c r="D141" s="4">
         <f t="shared" si="12"/>
         <v>9180</v>
       </c>
-      <c r="E141" s="7" t="str">
+      <c r="E141" s="6" t="str">
         <f t="shared" si="13"/>
         <v>23DC</v>
       </c>
-      <c r="F141" s="8"/>
-      <c r="G141" s="9">
+      <c r="F141" s="7"/>
+      <c r="G141" s="8">
         <f t="shared" si="14"/>
         <v>100</v>
       </c>
@@ -5425,35 +5422,35 @@
       <c r="C142" s="4">
         <v>0.8889</v>
       </c>
-      <c r="D142" s="5">
+      <c r="D142" s="4">
         <f t="shared" si="12"/>
         <v>8889</v>
       </c>
-      <c r="E142" s="7" t="str">
+      <c r="E142" s="6" t="str">
         <f t="shared" si="13"/>
         <v>22B9</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="9">
+      <c r="F142" s="7"/>
+      <c r="G142" s="8">
         <f t="shared" si="14"/>
         <v>101</v>
       </c>
-      <c r="H142" s="10"/>
+      <c r="H142" s="9"/>
     </row>
     <row r="143" spans="3:7">
-      <c r="C143" s="6">
+      <c r="C143" s="5">
         <v>0.8346</v>
       </c>
-      <c r="D143" s="5">
+      <c r="D143" s="4">
         <f t="shared" si="12"/>
         <v>8346</v>
       </c>
-      <c r="E143" s="7" t="str">
+      <c r="E143" s="6" t="str">
         <f t="shared" si="13"/>
         <v>209A</v>
       </c>
-      <c r="F143" s="8"/>
-      <c r="G143" s="9">
+      <c r="F143" s="7"/>
+      <c r="G143" s="8">
         <f t="shared" si="14"/>
         <v>102</v>
       </c>
@@ -5462,16 +5459,16 @@
       <c r="C144" s="4">
         <v>0.8099</v>
       </c>
-      <c r="D144" s="5">
+      <c r="D144" s="4">
         <f t="shared" si="12"/>
         <v>8099</v>
       </c>
-      <c r="E144" s="7" t="str">
+      <c r="E144" s="6" t="str">
         <f t="shared" si="13"/>
         <v>1FA3</v>
       </c>
-      <c r="F144" s="8"/>
-      <c r="G144" s="9">
+      <c r="F144" s="7"/>
+      <c r="G144" s="8">
         <f t="shared" si="14"/>
         <v>103</v>
       </c>
@@ -5480,16 +5477,16 @@
       <c r="C145" s="4">
         <v>0.787</v>
       </c>
-      <c r="D145" s="5">
+      <c r="D145" s="4">
         <f t="shared" si="12"/>
         <v>7870</v>
       </c>
-      <c r="E145" s="7" t="str">
+      <c r="E145" s="6" t="str">
         <f t="shared" si="13"/>
         <v>1EBE</v>
       </c>
-      <c r="F145" s="8"/>
-      <c r="G145" s="9">
+      <c r="F145" s="7"/>
+      <c r="G145" s="8">
         <f t="shared" si="14"/>
         <v>104</v>
       </c>
@@ -5498,16 +5495,16 @@
       <c r="C146" s="4">
         <v>0.7665</v>
       </c>
-      <c r="D146" s="5">
+      <c r="D146" s="4">
         <f t="shared" si="12"/>
         <v>7665</v>
       </c>
-      <c r="E146" s="7" t="str">
+      <c r="E146" s="6" t="str">
         <f t="shared" si="13"/>
         <v>1DF1</v>
       </c>
-      <c r="F146" s="8"/>
-      <c r="G146" s="9">
+      <c r="F146" s="7"/>
+      <c r="G146" s="8">
         <f t="shared" si="14"/>
         <v>105</v>
       </c>
@@ -5516,16 +5513,16 @@
       <c r="C147" s="4">
         <v>0.7485</v>
       </c>
-      <c r="D147" s="5">
+      <c r="D147" s="4">
         <f t="shared" si="12"/>
         <v>7485</v>
       </c>
-      <c r="E147" s="7" t="str">
+      <c r="E147" s="6" t="str">
         <f t="shared" si="13"/>
         <v>1D3D</v>
       </c>
-      <c r="F147" s="8"/>
-      <c r="G147" s="9">
+      <c r="F147" s="7"/>
+      <c r="G147" s="8">
         <f t="shared" si="14"/>
         <v>106</v>
       </c>
@@ -5534,34 +5531,34 @@
       <c r="C148" s="4">
         <v>0.7334</v>
       </c>
-      <c r="D148" s="5">
+      <c r="D148" s="4">
         <f t="shared" si="12"/>
         <v>7334</v>
       </c>
-      <c r="E148" s="7" t="str">
+      <c r="E148" s="6" t="str">
         <f t="shared" si="13"/>
         <v>1CA6</v>
       </c>
-      <c r="F148" s="8"/>
-      <c r="G148" s="9">
+      <c r="F148" s="7"/>
+      <c r="G148" s="8">
         <f t="shared" si="14"/>
         <v>107</v>
       </c>
     </row>
     <row r="149" spans="3:7">
-      <c r="C149" s="6">
+      <c r="C149" s="5">
         <v>0.7214</v>
       </c>
-      <c r="D149" s="5">
+      <c r="D149" s="4">
         <f t="shared" si="12"/>
         <v>7214</v>
       </c>
-      <c r="E149" s="7" t="str">
+      <c r="E149" s="6" t="str">
         <f t="shared" si="13"/>
         <v>1C2E</v>
       </c>
-      <c r="F149" s="8"/>
-      <c r="G149" s="9">
+      <c r="F149" s="7"/>
+      <c r="G149" s="8">
         <f t="shared" si="14"/>
         <v>108</v>
       </c>
@@ -5570,16 +5567,16 @@
       <c r="C150" s="4">
         <v>0.713</v>
       </c>
-      <c r="D150" s="5">
+      <c r="D150" s="4">
         <f t="shared" si="12"/>
         <v>7130</v>
       </c>
-      <c r="E150" s="7" t="str">
+      <c r="E150" s="6" t="str">
         <f t="shared" si="13"/>
         <v>1BDA</v>
       </c>
-      <c r="F150" s="8"/>
-      <c r="G150" s="9">
+      <c r="F150" s="7"/>
+      <c r="G150" s="8">
         <f t="shared" si="14"/>
         <v>109</v>
       </c>
@@ -5596,8 +5593,8 @@
   <sheetPr/>
   <dimension ref="C4:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>

</xml_diff>